<commit_message>
mise à jour BOM cartes 2013.xlsx
</commit_message>
<xml_diff>
--- a/Elec/2013/BOM cartes 2013.xlsx
+++ b/Elec/2013/BOM cartes 2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19440" windowHeight="8505" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19440" windowHeight="8505" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Carte alimentation" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="364">
   <si>
     <t>produit</t>
   </si>
@@ -1627,6 +1627,9 @@
   </si>
   <si>
     <t>référence</t>
+  </si>
+  <si>
+    <t>Manquants</t>
   </si>
 </sst>
 </file>
@@ -1830,7 +1833,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1972,12 +1975,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="70">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
@@ -2935,118 +2944,118 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:K34" totalsRowShown="0" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:K34" totalsRowShown="0" dataDxfId="69">
   <autoFilter ref="A1:K34"/>
   <tableColumns count="11">
-    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="67"/>
-    <tableColumn id="1" name="produit" dataDxfId="66"/>
-    <tableColumn id="2" name="fabricant" dataDxfId="65"/>
-    <tableColumn id="3" name="ref fabriquant" dataDxfId="64"/>
-    <tableColumn id="4" name="fournisseur" dataDxfId="63"/>
-    <tableColumn id="5" name="ref fournisseur" dataDxfId="62"/>
-    <tableColumn id="6" name="MOQ" dataDxfId="61"/>
-    <tableColumn id="10" name="Quantité commande" dataDxfId="60"/>
-    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="59" dataCellStyle="Monétaire"/>
-    <tableColumn id="8" name="Prix total" dataDxfId="58" dataCellStyle="Monétaire">
+    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="68"/>
+    <tableColumn id="1" name="produit" dataDxfId="67"/>
+    <tableColumn id="2" name="fabricant" dataDxfId="66"/>
+    <tableColumn id="3" name="ref fabriquant" dataDxfId="65"/>
+    <tableColumn id="4" name="fournisseur" dataDxfId="64"/>
+    <tableColumn id="5" name="ref fournisseur" dataDxfId="63"/>
+    <tableColumn id="6" name="MOQ" dataDxfId="62"/>
+    <tableColumn id="10" name="Quantité commande" dataDxfId="61"/>
+    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="60" dataCellStyle="Monétaire"/>
+    <tableColumn id="8" name="Prix total" dataDxfId="59" dataCellStyle="Monétaire">
       <calculatedColumnFormula>Tableau2[[#This Row],[Prix unitaire HT]]*Tableau2[[#This Row],[Quantité commande]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Remarques" dataDxfId="57"/>
+    <tableColumn id="7" name="Remarques" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau22" displayName="Tableau22" ref="A1:K35" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau22" displayName="Tableau22" ref="A1:K35" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A1:K35"/>
   <tableColumns count="11">
-    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="55"/>
-    <tableColumn id="1" name="produit" dataDxfId="54"/>
-    <tableColumn id="2" name="fabricant" dataDxfId="53"/>
-    <tableColumn id="3" name="ref fabriquant" dataDxfId="52"/>
-    <tableColumn id="4" name="fournisseur" dataDxfId="51"/>
-    <tableColumn id="5" name="ref fournisseur" dataDxfId="50"/>
-    <tableColumn id="6" name="MOQ" dataDxfId="49"/>
-    <tableColumn id="10" name="Quantité commande" dataDxfId="48"/>
-    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="47" dataCellStyle="Monétaire"/>
-    <tableColumn id="8" name="Prix total" dataDxfId="46" dataCellStyle="Monétaire">
+    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="56"/>
+    <tableColumn id="1" name="produit" dataDxfId="55"/>
+    <tableColumn id="2" name="fabricant" dataDxfId="54"/>
+    <tableColumn id="3" name="ref fabriquant" dataDxfId="53"/>
+    <tableColumn id="4" name="fournisseur" dataDxfId="52"/>
+    <tableColumn id="5" name="ref fournisseur" dataDxfId="51"/>
+    <tableColumn id="6" name="MOQ" dataDxfId="50"/>
+    <tableColumn id="10" name="Quantité commande" dataDxfId="49"/>
+    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="48" dataCellStyle="Monétaire"/>
+    <tableColumn id="8" name="Prix total" dataDxfId="47" dataCellStyle="Monétaire">
       <calculatedColumnFormula>Tableau22[[#This Row],[Prix unitaire HT]]*Tableau22[[#This Row],[Quantité commande]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Remarques" dataDxfId="45"/>
+    <tableColumn id="7" name="Remarques" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau224" displayName="Tableau224" ref="A1:K11" totalsRowShown="0" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau224" displayName="Tableau224" ref="A1:K11" totalsRowShown="0" dataDxfId="45">
   <autoFilter ref="A1:K11"/>
   <tableColumns count="11">
-    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="43"/>
-    <tableColumn id="1" name="produit" dataDxfId="42"/>
-    <tableColumn id="2" name="fabricant" dataDxfId="41"/>
-    <tableColumn id="3" name="ref fabriquant" dataDxfId="40"/>
-    <tableColumn id="4" name="fournisseur" dataDxfId="39"/>
-    <tableColumn id="5" name="ref fournisseur" dataDxfId="38"/>
-    <tableColumn id="6" name="MOQ" dataDxfId="37"/>
-    <tableColumn id="10" name="Quantité commande" dataDxfId="36"/>
-    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="35" dataCellStyle="Monétaire"/>
-    <tableColumn id="8" name="Prix total" dataDxfId="34" dataCellStyle="Monétaire">
+    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="44"/>
+    <tableColumn id="1" name="produit" dataDxfId="43"/>
+    <tableColumn id="2" name="fabricant" dataDxfId="42"/>
+    <tableColumn id="3" name="ref fabriquant" dataDxfId="41"/>
+    <tableColumn id="4" name="fournisseur" dataDxfId="40"/>
+    <tableColumn id="5" name="ref fournisseur" dataDxfId="39"/>
+    <tableColumn id="6" name="MOQ" dataDxfId="38"/>
+    <tableColumn id="10" name="Quantité commande" dataDxfId="37"/>
+    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="36" dataCellStyle="Monétaire"/>
+    <tableColumn id="8" name="Prix total" dataDxfId="35" dataCellStyle="Monétaire">
       <calculatedColumnFormula>Tableau224[[#This Row],[Prix unitaire HT]]*Tableau224[[#This Row],[Quantité commande]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Remarques" dataDxfId="33"/>
+    <tableColumn id="7" name="Remarques" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau2245" displayName="Tableau2245" ref="A1:K48" totalsRowShown="0" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau2245" displayName="Tableau2245" ref="A1:K48" totalsRowShown="0" dataDxfId="33">
   <autoFilter ref="A1:K48"/>
   <tableColumns count="11">
-    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="31"/>
-    <tableColumn id="1" name="produit" dataDxfId="30"/>
-    <tableColumn id="2" name="fabricant" dataDxfId="29"/>
-    <tableColumn id="3" name="ref fabriquant" dataDxfId="28"/>
-    <tableColumn id="4" name="fournisseur" dataDxfId="27"/>
-    <tableColumn id="5" name="ref fournisseur" dataDxfId="26"/>
-    <tableColumn id="6" name="MOQ" dataDxfId="25"/>
-    <tableColumn id="10" name="Quantité commande" dataDxfId="24"/>
-    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="23" dataCellStyle="Monétaire"/>
-    <tableColumn id="8" name="Prix total" dataDxfId="22" dataCellStyle="Monétaire">
+    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="32"/>
+    <tableColumn id="1" name="produit" dataDxfId="31"/>
+    <tableColumn id="2" name="fabricant" dataDxfId="30"/>
+    <tableColumn id="3" name="ref fabriquant" dataDxfId="29"/>
+    <tableColumn id="4" name="fournisseur" dataDxfId="28"/>
+    <tableColumn id="5" name="ref fournisseur" dataDxfId="27"/>
+    <tableColumn id="6" name="MOQ" dataDxfId="26"/>
+    <tableColumn id="10" name="Quantité commande" dataDxfId="25"/>
+    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="24" dataCellStyle="Monétaire"/>
+    <tableColumn id="8" name="Prix total" dataDxfId="23" dataCellStyle="Monétaire">
       <calculatedColumnFormula>Tableau2245[[#This Row],[Prix unitaire HT]]*Tableau2245[[#This Row],[Quantité commande]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Remarques" dataDxfId="21"/>
+    <tableColumn id="7" name="Remarques" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau22457" displayName="Tableau22457" ref="A1:K48" totalsRowShown="0" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau22457" displayName="Tableau22457" ref="A1:K48" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="A1:K48"/>
   <tableColumns count="11">
-    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="19"/>
-    <tableColumn id="1" name="produit" dataDxfId="18"/>
-    <tableColumn id="2" name="fabricant" dataDxfId="17"/>
-    <tableColumn id="3" name="ref fabriquant" dataDxfId="16"/>
-    <tableColumn id="4" name="fournisseur" dataDxfId="15"/>
-    <tableColumn id="5" name="ref fournisseur" dataDxfId="14"/>
-    <tableColumn id="6" name="MOQ" dataDxfId="13"/>
-    <tableColumn id="10" name="Quantité commande" dataDxfId="12"/>
-    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="11" dataCellStyle="Monétaire"/>
-    <tableColumn id="8" name="Prix total" dataDxfId="10" dataCellStyle="Monétaire">
+    <tableColumn id="23" name="Quantité sur la carte" dataDxfId="20"/>
+    <tableColumn id="1" name="produit" dataDxfId="19"/>
+    <tableColumn id="2" name="fabricant" dataDxfId="18"/>
+    <tableColumn id="3" name="ref fabriquant" dataDxfId="17"/>
+    <tableColumn id="4" name="fournisseur" dataDxfId="16"/>
+    <tableColumn id="5" name="ref fournisseur" dataDxfId="15"/>
+    <tableColumn id="6" name="MOQ" dataDxfId="14"/>
+    <tableColumn id="10" name="Quantité commande" dataDxfId="13"/>
+    <tableColumn id="9" name="Prix unitaire HT" dataDxfId="12" dataCellStyle="Monétaire"/>
+    <tableColumn id="8" name="Prix total" dataDxfId="11" dataCellStyle="Monétaire">
       <calculatedColumnFormula>Tableau22457[[#This Row],[Prix unitaire HT]]*Tableau22457[[#This Row],[Quantité commande]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Remarques" dataDxfId="9"/>
+    <tableColumn id="7" name="Remarques" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A5:T199" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A5:T199">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A5:U199" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A5:U199">
     <filterColumn colId="12">
       <filters blank="1">
         <filter val="1"/>
@@ -3076,46 +3085,38 @@
         <filter val="9"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="15">
-      <filters>
-        <filter val="10"/>
-        <filter val="15"/>
-        <filter val="20"/>
-        <filter val="30"/>
-        <filter val="35"/>
-        <filter val="5"/>
-        <filter val="6"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <sortState ref="A6:T187">
     <sortCondition ref="G6:G187"/>
   </sortState>
-  <tableColumns count="20">
+  <tableColumns count="21">
     <tableColumn id="1" name="Quantité sur la carte alimentation"/>
     <tableColumn id="2" name="Quantité sur la carte connectique CM"/>
     <tableColumn id="3" name="Quantité sur la carte support couleur"/>
     <tableColumn id="4" name="Quantité sur la carte mère"/>
     <tableColumn id="16" name="Quantité sur carte hacheur"/>
-    <tableColumn id="18" name="Quantité pour cablage" dataDxfId="7"/>
+    <tableColumn id="18" name="Quantité pour cablage" dataDxfId="8"/>
     <tableColumn id="5" name="produit"/>
     <tableColumn id="6" name="fabricant"/>
     <tableColumn id="7" name="ref fabriquant"/>
     <tableColumn id="8" name="fournisseur"/>
-    <tableColumn id="9" name="ref fournisseur" dataDxfId="6"/>
+    <tableColumn id="9" name="ref fournisseur" dataDxfId="7"/>
     <tableColumn id="10" name="MOQ"/>
-    <tableColumn id="17" name="Besoin" dataDxfId="5">
+    <tableColumn id="17" name="Besoin" dataDxfId="6">
       <calculatedColumnFormula>SUMPRODUCT($A$2:$F$2,Tableau5[[#This Row],[Quantité sur la carte alimentation]:[Quantité pour cablage]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Prix unitaire HT" dataDxfId="4" dataCellStyle="Monétaire"/>
-    <tableColumn id="21" name="Stock de Oufff" dataDxfId="3" dataCellStyle="Monétaire"/>
+    <tableColumn id="20" name="Prix unitaire HT" dataDxfId="5" dataCellStyle="Monétaire"/>
+    <tableColumn id="21" name="Stock de Oufff" dataDxfId="4" dataCellStyle="Monétaire"/>
     <tableColumn id="11" name="Quantité à commander"/>
-    <tableColumn id="15" name="Quantité commandée" dataDxfId="2"/>
-    <tableColumn id="19" name="Quantité reçue" dataDxfId="1"/>
-    <tableColumn id="13" name="Prix total" dataDxfId="0">
+    <tableColumn id="15" name="Quantité commandée" dataDxfId="3"/>
+    <tableColumn id="19" name="Quantité reçue" dataDxfId="2"/>
+    <tableColumn id="13" name="Prix total" dataDxfId="1">
       <calculatedColumnFormula>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" name="Remarques"/>
+    <tableColumn id="12" name="Manquants" dataDxfId="0">
+      <calculatedColumnFormula>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3410,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7536,14 +7537,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T199"/>
+  <dimension ref="A1:U199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="G1" sqref="G1"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
-      <selection pane="bottomRight" activeCell="Q200" sqref="Q200"/>
+    <sheetView tabSelected="1" topLeftCell="F71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7554,7 +7551,7 @@
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="55.140625" customWidth="1"/>
+    <col min="7" max="7" width="45" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
@@ -7568,7 +7565,7 @@
     <col min="19" max="20" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>160</v>
       </c>
@@ -7580,7 +7577,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="32">
         <v>3</v>
       </c>
@@ -7600,7 +7597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>154</v>
       </c>
@@ -7661,8 +7658,11 @@
       <c r="T5" s="36" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="69" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="20">
         <v>16</v>
@@ -7701,14 +7701,20 @@
       <c r="Q6" s="20">
         <v>100</v>
       </c>
-      <c r="R6" s="20"/>
+      <c r="R6" s="20">
+        <v>100</v>
+      </c>
       <c r="S6" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0.8</v>
       </c>
       <c r="T6" s="20"/>
-    </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="20">
         <v>16</v>
@@ -7751,8 +7757,12 @@
         <v>0</v>
       </c>
       <c r="T7" s="20"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="20">
         <v>16</v>
@@ -7795,8 +7805,12 @@
         <v>0</v>
       </c>
       <c r="T8" s="20"/>
-    </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -7837,8 +7851,12 @@
         <v>0</v>
       </c>
       <c r="T9" s="20"/>
-    </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -7879,8 +7897,12 @@
         <v>0</v>
       </c>
       <c r="T10" s="20"/>
-    </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -7917,8 +7939,12 @@
         <v>0</v>
       </c>
       <c r="T11" s="20"/>
-    </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="20">
         <v>4</v>
@@ -7963,8 +7989,12 @@
         <v>0</v>
       </c>
       <c r="T12" s="20"/>
-    </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="20">
         <v>4</v>
@@ -8009,8 +8039,12 @@
         <v>0</v>
       </c>
       <c r="T13" s="20"/>
-    </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="20">
         <v>4</v>
@@ -8053,8 +8087,12 @@
         <v>0</v>
       </c>
       <c r="T14" s="20"/>
-    </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="20">
         <v>11</v>
@@ -8095,14 +8133,20 @@
       <c r="Q15" s="20">
         <v>200</v>
       </c>
-      <c r="R15" s="20"/>
+      <c r="R15" s="20">
+        <v>200</v>
+      </c>
       <c r="S15" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1.6</v>
       </c>
       <c r="T15" s="20"/>
-    </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="20">
         <v>11</v>
@@ -8145,8 +8189,12 @@
         <v>0</v>
       </c>
       <c r="T16" s="20"/>
-    </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="20">
         <v>11</v>
@@ -8191,8 +8239,12 @@
         <v>0</v>
       </c>
       <c r="T17" s="20"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -8233,8 +8285,12 @@
         <v>0</v>
       </c>
       <c r="T18" s="20"/>
-    </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
@@ -8271,8 +8327,12 @@
         <v>0</v>
       </c>
       <c r="T19" s="20"/>
-    </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -8313,8 +8373,12 @@
         <v>0</v>
       </c>
       <c r="T20" s="20"/>
-    </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -8351,8 +8415,12 @@
         <v>0</v>
       </c>
       <c r="T21" s="20"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -8389,14 +8457,20 @@
       <c r="Q22" s="20">
         <v>10</v>
       </c>
-      <c r="R22" s="20"/>
+      <c r="R22" s="20">
+        <v>10</v>
+      </c>
       <c r="S22" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>3.3000000000000003</v>
       </c>
       <c r="T22" s="20"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -8437,8 +8511,12 @@
         <v>0</v>
       </c>
       <c r="T23" s="20"/>
-    </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -8479,8 +8557,12 @@
         <v>0</v>
       </c>
       <c r="T24" s="20"/>
-    </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -8517,8 +8599,12 @@
         <v>0</v>
       </c>
       <c r="T25" s="20"/>
-    </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -8559,8 +8645,12 @@
         <v>0</v>
       </c>
       <c r="T26" s="20"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -8601,8 +8691,12 @@
         <v>0</v>
       </c>
       <c r="T27" s="20"/>
-    </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -8639,14 +8733,20 @@
       <c r="Q28" s="20">
         <v>25</v>
       </c>
-      <c r="R28" s="20"/>
+      <c r="R28" s="20">
+        <v>25</v>
+      </c>
       <c r="S28" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>6.1</v>
       </c>
       <c r="T28" s="20"/>
-    </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -8687,8 +8787,12 @@
         <v>0</v>
       </c>
       <c r="T29" s="20"/>
-    </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
@@ -8729,8 +8833,12 @@
         <v>0</v>
       </c>
       <c r="T30" s="20"/>
-    </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
@@ -8767,8 +8875,12 @@
         <v>0</v>
       </c>
       <c r="T31" s="20"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="20">
         <v>2</v>
@@ -8809,8 +8921,12 @@
         <v>0</v>
       </c>
       <c r="T32" s="20"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>6</v>
       </c>
@@ -8851,14 +8967,20 @@
       <c r="Q33" s="20">
         <v>20</v>
       </c>
-      <c r="R33" s="20"/>
+      <c r="R33" s="20">
+        <v>20</v>
+      </c>
       <c r="S33" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>5.84</v>
       </c>
       <c r="T33" s="20"/>
-    </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <v>6</v>
       </c>
@@ -8899,8 +9021,12 @@
         <v>0</v>
       </c>
       <c r="T34" s="20"/>
-    </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>6</v>
       </c>
@@ -8939,8 +9065,12 @@
         <v>0</v>
       </c>
       <c r="T35" s="20"/>
-    </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -8986,8 +9116,12 @@
         <v>0</v>
       </c>
       <c r="T36" s="20"/>
-    </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -9026,14 +9160,20 @@
       <c r="Q37" s="20">
         <v>12</v>
       </c>
-      <c r="R37" s="20"/>
+      <c r="R37" s="20">
+        <v>12</v>
+      </c>
       <c r="S37" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>6.36</v>
       </c>
       <c r="T37" s="20"/>
-    </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U37">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -9078,8 +9218,12 @@
         <v>0</v>
       </c>
       <c r="T38" s="20"/>
-    </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U38">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
@@ -9120,14 +9264,20 @@
       <c r="Q39" s="20">
         <v>2</v>
       </c>
-      <c r="R39" s="20"/>
+      <c r="R39" s="20">
+        <v>2</v>
+      </c>
       <c r="S39" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>21.28</v>
       </c>
       <c r="T39" s="20"/>
-    </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U39">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="20">
         <v>5</v>
@@ -9172,8 +9322,12 @@
         <v>0</v>
       </c>
       <c r="T40" s="20"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U40">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
       <c r="B41" s="20">
         <v>5</v>
@@ -9214,14 +9368,20 @@
       <c r="Q41" s="20">
         <v>5</v>
       </c>
-      <c r="R41" s="20"/>
+      <c r="R41" s="20">
+        <v>5</v>
+      </c>
       <c r="S41" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>9.5499999999999989</v>
       </c>
       <c r="T41" s="20"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U41">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
       <c r="B42" s="20">
         <v>5</v>
@@ -9264,8 +9424,12 @@
         <v>0</v>
       </c>
       <c r="T42" s="20"/>
-    </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U42">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -9306,8 +9470,12 @@
         <v>0</v>
       </c>
       <c r="T43" s="20"/>
-    </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U43">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
@@ -9348,8 +9516,12 @@
         <v>0</v>
       </c>
       <c r="T44" s="20"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U44">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
@@ -9386,14 +9558,20 @@
       <c r="Q45" s="20">
         <v>5</v>
       </c>
-      <c r="R45" s="20"/>
+      <c r="R45" s="20">
+        <v>5</v>
+      </c>
       <c r="S45" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1</v>
       </c>
       <c r="T45" s="20"/>
-    </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U45">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="20"/>
       <c r="B46" s="20">
         <v>1</v>
@@ -9428,8 +9606,12 @@
         <v>0</v>
       </c>
       <c r="T46" s="20"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U46">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
       <c r="B47" s="20">
         <v>1</v>
@@ -9466,14 +9648,20 @@
       <c r="Q47" s="20">
         <v>5</v>
       </c>
-      <c r="R47" s="20"/>
+      <c r="R47" s="20">
+        <v>5</v>
+      </c>
       <c r="S47" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1.1100000000000001</v>
       </c>
       <c r="T47" s="20"/>
-    </row>
-    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U47">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
       <c r="B48" s="20">
         <v>1</v>
@@ -9510,8 +9698,12 @@
         <v>0</v>
       </c>
       <c r="T48" s="20"/>
-    </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U48">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
@@ -9547,7 +9739,9 @@
       <c r="Q49" s="20">
         <v>2</v>
       </c>
-      <c r="R49" s="20"/>
+      <c r="R49" s="20">
+        <v>2</v>
+      </c>
       <c r="S49" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>7.66</v>
@@ -9555,8 +9749,12 @@
       <c r="T49" s="20" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U49">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="20">
         <v>3</v>
@@ -9591,8 +9789,12 @@
         <v>0</v>
       </c>
       <c r="T50" s="20"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U50">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="20"/>
       <c r="B51" s="20">
         <v>3</v>
@@ -9629,14 +9831,20 @@
       <c r="Q51" s="20">
         <v>10</v>
       </c>
-      <c r="R51" s="20"/>
+      <c r="R51" s="20">
+        <v>10</v>
+      </c>
       <c r="S51" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1.1600000000000001</v>
       </c>
       <c r="T51" s="20"/>
-    </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U51">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="20"/>
       <c r="B52" s="20">
         <v>3</v>
@@ -9673,8 +9881,12 @@
         <v>0</v>
       </c>
       <c r="T52" s="20"/>
-    </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U52">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
@@ -9711,8 +9923,12 @@
         <v>0</v>
       </c>
       <c r="T53" s="20"/>
-    </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U53">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
@@ -9751,8 +9967,12 @@
         <v>0</v>
       </c>
       <c r="T54" s="20"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U54">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
@@ -9793,8 +10013,12 @@
         <v>0</v>
       </c>
       <c r="T55" s="20"/>
-    </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U55">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
@@ -9833,8 +10057,12 @@
         <v>0</v>
       </c>
       <c r="T56" s="20"/>
-    </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U56">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <v>4</v>
       </c>
@@ -9860,15 +10088,23 @@
       <c r="N57" s="27"/>
       <c r="O57" s="45"/>
       <c r="P57" s="20"/>
-      <c r="Q57" s="20"/>
-      <c r="R57" s="20"/>
+      <c r="Q57" s="20">
+        <v>12</v>
+      </c>
+      <c r="R57" s="20">
+        <v>12</v>
+      </c>
       <c r="S57" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T57" s="20"/>
-    </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U57">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
@@ -9911,8 +10147,12 @@
         <v>0</v>
       </c>
       <c r="T58" s="20"/>
-    </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U58">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
@@ -9955,8 +10195,12 @@
         <v>0</v>
       </c>
       <c r="T59" s="20"/>
-    </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U59">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="C60" s="20"/>
@@ -9995,14 +10239,20 @@
       <c r="Q60" s="20">
         <v>2</v>
       </c>
-      <c r="R60" s="20"/>
+      <c r="R60" s="20">
+        <v>2</v>
+      </c>
       <c r="S60" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1.9</v>
       </c>
       <c r="T60" s="20"/>
-    </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U60">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="C61" s="20"/>
@@ -10041,8 +10291,12 @@
         <v>0</v>
       </c>
       <c r="T61" s="20"/>
-    </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U61">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
         <v>2</v>
       </c>
@@ -10092,8 +10346,12 @@
         <v>0</v>
       </c>
       <c r="T62" s="20"/>
-    </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U62">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>2</v>
       </c>
@@ -10142,8 +10400,12 @@
         <v>0</v>
       </c>
       <c r="T63" s="20"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U63">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
         <v>2</v>
       </c>
@@ -10184,7 +10446,9 @@
       <c r="Q64" s="20">
         <v>30</v>
       </c>
-      <c r="R64" s="20"/>
+      <c r="R64" s="20">
+        <v>30</v>
+      </c>
       <c r="S64" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>6</v>
@@ -10192,8 +10456,12 @@
       <c r="T64" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U64">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="20">
         <v>4</v>
       </c>
@@ -10242,8 +10510,12 @@
         <v>0</v>
       </c>
       <c r="T65" s="20"/>
-    </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U65">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="20">
         <v>4</v>
       </c>
@@ -10275,7 +10547,7 @@
         <v>48</v>
       </c>
       <c r="N66" s="27">
-        <v>0.86</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="O66" s="45">
         <v>19</v>
@@ -10290,8 +10562,12 @@
         <v>0</v>
       </c>
       <c r="T66" s="20"/>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U66">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="20">
         <v>4</v>
       </c>
@@ -10330,7 +10606,9 @@
       <c r="Q67" s="20">
         <v>35</v>
       </c>
-      <c r="R67" s="20"/>
+      <c r="R67" s="20">
+        <v>0</v>
+      </c>
       <c r="S67" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>7</v>
@@ -10338,8 +10616,12 @@
       <c r="T67" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U67">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="20"/>
       <c r="B68" s="20">
         <v>3</v>
@@ -10390,8 +10672,12 @@
         <v>0</v>
       </c>
       <c r="T68" s="20"/>
-    </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U68">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="20"/>
       <c r="B69" s="20">
         <v>3</v>
@@ -10440,8 +10726,12 @@
         <v>0</v>
       </c>
       <c r="T69" s="20"/>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U69">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="20"/>
       <c r="B70" s="20">
         <v>3</v>
@@ -10482,7 +10772,9 @@
       <c r="Q70" s="20">
         <v>15</v>
       </c>
-      <c r="R70" s="20"/>
+      <c r="R70" s="20">
+        <v>15</v>
+      </c>
       <c r="S70" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>3</v>
@@ -10490,8 +10782,12 @@
       <c r="T70" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U70">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="20"/>
       <c r="B71" s="20">
         <v>5</v>
@@ -10540,8 +10836,12 @@
         <v>0</v>
       </c>
       <c r="T71" s="20"/>
-    </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U71">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="20"/>
       <c r="B72" s="20">
         <v>5</v>
@@ -10588,8 +10888,12 @@
         <v>0</v>
       </c>
       <c r="T72" s="20"/>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U72">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="20"/>
       <c r="B73" s="20">
         <v>5</v>
@@ -10628,7 +10932,9 @@
       <c r="Q73" s="20">
         <v>20</v>
       </c>
-      <c r="R73" s="20"/>
+      <c r="R73" s="20">
+        <v>20</v>
+      </c>
       <c r="S73" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>5</v>
@@ -10636,8 +10942,12 @@
       <c r="T73" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U73">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
       <c r="C74" s="20">
@@ -10678,8 +10988,12 @@
         <v>0</v>
       </c>
       <c r="T74" s="20"/>
-    </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U74">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="C75" s="20">
@@ -10718,8 +11032,12 @@
         <v>0</v>
       </c>
       <c r="T75" s="20"/>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U75">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
       <c r="C76" s="20">
@@ -10754,7 +11072,9 @@
       <c r="Q76" s="20">
         <v>15</v>
       </c>
-      <c r="R76" s="20"/>
+      <c r="R76" s="20">
+        <v>15</v>
+      </c>
       <c r="S76" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>3.75</v>
@@ -10762,8 +11082,12 @@
       <c r="T76" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U76">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="20"/>
       <c r="B77" s="20">
         <v>2</v>
@@ -10804,8 +11128,12 @@
         <v>0</v>
       </c>
       <c r="T77" s="20"/>
-    </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U77">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
         <v>2</v>
       </c>
@@ -10854,8 +11182,12 @@
         <v>0</v>
       </c>
       <c r="T78" s="20"/>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U78">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
         <v>2</v>
       </c>
@@ -10896,14 +11228,20 @@
       <c r="Q79" s="20">
         <v>5</v>
       </c>
-      <c r="R79" s="20"/>
+      <c r="R79" s="20">
+        <v>10</v>
+      </c>
       <c r="S79" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T79" s="20"/>
-    </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U79">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>2</v>
       </c>
@@ -10946,8 +11284,12 @@
         <v>0</v>
       </c>
       <c r="T80" s="20"/>
-    </row>
-    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U80">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
       <c r="B81" s="20"/>
       <c r="C81" s="20"/>
@@ -10984,8 +11326,12 @@
         <v>0</v>
       </c>
       <c r="T81" s="20"/>
-    </row>
-    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U81">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
       <c r="C82" s="20"/>
@@ -11031,8 +11377,12 @@
         <v>0</v>
       </c>
       <c r="T82" s="20"/>
-    </row>
-    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U82">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
       <c r="C83" s="20"/>
@@ -11071,14 +11421,20 @@
       <c r="Q83" s="20">
         <v>12</v>
       </c>
-      <c r="R83" s="20"/>
+      <c r="R83" s="20">
+        <v>12</v>
+      </c>
       <c r="S83" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>28.08</v>
       </c>
       <c r="T83" s="20"/>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U83">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
         <v>2</v>
       </c>
@@ -11117,14 +11473,20 @@
       <c r="Q84" s="20">
         <v>5</v>
       </c>
-      <c r="R84" s="20"/>
+      <c r="R84" s="20">
+        <v>10</v>
+      </c>
       <c r="S84" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T84" s="20"/>
-    </row>
-    <row r="85" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U84">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
         <v>2</v>
       </c>
@@ -11167,8 +11529,12 @@
         <v>0</v>
       </c>
       <c r="T85" s="20"/>
-    </row>
-    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U85">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
       <c r="C86" s="20"/>
@@ -11211,8 +11577,12 @@
         <v>0</v>
       </c>
       <c r="T86" s="20"/>
-    </row>
-    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U86">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="20"/>
       <c r="B87" s="20"/>
       <c r="C87" s="20"/>
@@ -11251,14 +11621,20 @@
       <c r="Q87" s="20">
         <v>2</v>
       </c>
-      <c r="R87" s="20"/>
+      <c r="R87" s="20">
+        <v>2</v>
+      </c>
       <c r="S87" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1.24</v>
       </c>
       <c r="T87" s="20"/>
-    </row>
-    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U87">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
       <c r="C88" s="20"/>
@@ -11297,8 +11673,12 @@
         <v>0</v>
       </c>
       <c r="T88" s="20"/>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U88">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="20"/>
       <c r="B89" s="20"/>
       <c r="C89" s="20"/>
@@ -11334,14 +11714,20 @@
       <c r="Q89" s="20">
         <v>10</v>
       </c>
-      <c r="R89" s="20"/>
+      <c r="R89" s="20">
+        <v>10</v>
+      </c>
       <c r="S89" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>6</v>
       </c>
       <c r="T89" s="20"/>
-    </row>
-    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U89">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
       <c r="C90" s="20"/>
@@ -11382,8 +11768,12 @@
         <v>0</v>
       </c>
       <c r="T90" s="20"/>
-    </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U90">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="20"/>
       <c r="B91" s="20"/>
       <c r="C91" s="20"/>
@@ -11420,14 +11810,20 @@
       <c r="Q91" s="20">
         <v>5</v>
       </c>
-      <c r="R91" s="20"/>
+      <c r="R91" s="20">
+        <v>5</v>
+      </c>
       <c r="S91" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>3.75</v>
       </c>
       <c r="T91" s="20"/>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U91">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
       <c r="C92" s="20"/>
@@ -11462,14 +11858,20 @@
       <c r="Q92" s="20">
         <v>20</v>
       </c>
-      <c r="R92" s="20"/>
+      <c r="R92" s="20">
+        <v>0</v>
+      </c>
       <c r="S92" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>17</v>
       </c>
       <c r="T92" s="20"/>
-    </row>
-    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U92">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="20">
         <v>7</v>
       </c>
@@ -11500,8 +11902,12 @@
         <v>0</v>
       </c>
       <c r="T93" s="20"/>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U93">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="C94" s="20"/>
@@ -11546,8 +11952,12 @@
         <v>0</v>
       </c>
       <c r="T94" s="20"/>
-    </row>
-    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U94">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="C95" s="20"/>
@@ -11588,8 +11998,12 @@
         <v>0</v>
       </c>
       <c r="T95" s="20"/>
-    </row>
-    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U95">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="C96" s="20"/>
@@ -11630,8 +12044,12 @@
         <v>0</v>
       </c>
       <c r="T96" s="20"/>
-    </row>
-    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U96">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="C97" s="20"/>
@@ -11670,14 +12088,20 @@
       <c r="Q97" s="20">
         <v>5</v>
       </c>
-      <c r="R97" s="20"/>
+      <c r="R97" s="20">
+        <v>5</v>
+      </c>
       <c r="S97" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>3.6960000000000002</v>
       </c>
       <c r="T97" s="20"/>
-    </row>
-    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U97">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="C98" s="20"/>
@@ -11720,10 +12144,14 @@
         <v>0</v>
       </c>
       <c r="T98" s="20"/>
-    </row>
-    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U98">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B99" s="20"/>
       <c r="C99" s="20"/>
@@ -11744,7 +12172,7 @@
       <c r="L99" s="20"/>
       <c r="M99" s="20">
         <f>SUMPRODUCT($A$2:$F$2,Tableau5[[#This Row],[Quantité sur la carte alimentation]:[Quantité pour cablage]])</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N99" s="27"/>
       <c r="O99" s="45"/>
@@ -11758,10 +12186,14 @@
         <v>0</v>
       </c>
       <c r="T99" s="20"/>
-    </row>
-    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U99">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B100" s="20"/>
       <c r="C100" s="20"/>
@@ -11788,7 +12220,7 @@
       </c>
       <c r="M100" s="20">
         <f>SUMPRODUCT($A$2:$F$2,Tableau5[[#This Row],[Quantité sur la carte alimentation]:[Quantité pour cablage]])</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N100" s="27">
         <v>7.66</v>
@@ -11804,10 +12236,14 @@
         <v>0</v>
       </c>
       <c r="T100" s="20"/>
-    </row>
-    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U100">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B101" s="20"/>
       <c r="C101" s="20"/>
@@ -11832,28 +12268,34 @@
       <c r="L101" s="20"/>
       <c r="M101" s="20">
         <f>SUMPRODUCT($A$2:$F$2,Tableau5[[#This Row],[Quantité sur la carte alimentation]:[Quantité pour cablage]])</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N101" s="27">
         <v>7.97</v>
       </c>
       <c r="O101" s="45"/>
       <c r="P101" s="20">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q101" s="20">
         <v>7</v>
       </c>
-      <c r="R101" s="20"/>
+      <c r="R101" s="20">
+        <v>7</v>
+      </c>
       <c r="S101" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
-        <v>55.79</v>
+        <v>79.7</v>
       </c>
       <c r="T101" s="20"/>
-    </row>
-    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U101">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B102" s="20"/>
       <c r="C102" s="20"/>
@@ -11874,7 +12316,7 @@
       <c r="L102" s="20"/>
       <c r="M102" s="20">
         <f>SUMPRODUCT($A$2:$F$2,Tableau5[[#This Row],[Quantité sur la carte alimentation]:[Quantité pour cablage]])</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N102" s="27"/>
       <c r="O102" s="45"/>
@@ -11888,8 +12330,12 @@
         <v>0</v>
       </c>
       <c r="T102" s="20"/>
-    </row>
-    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U102">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="20">
         <v>1</v>
       </c>
@@ -11926,8 +12372,12 @@
         <v>0</v>
       </c>
       <c r="T103" s="20"/>
-    </row>
-    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U103">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="20">
         <v>1</v>
       </c>
@@ -11964,8 +12414,12 @@
         <v>0</v>
       </c>
       <c r="T104" s="20"/>
-    </row>
-    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U104">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="20">
         <v>1</v>
       </c>
@@ -12004,14 +12458,20 @@
       <c r="Q105" s="20">
         <v>4</v>
       </c>
-      <c r="R105" s="20"/>
+      <c r="R105" s="20">
+        <v>4</v>
+      </c>
       <c r="S105" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>4.12</v>
       </c>
       <c r="T105" s="20"/>
-    </row>
-    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U105">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="20">
         <v>1</v>
       </c>
@@ -12054,8 +12514,12 @@
         <v>0</v>
       </c>
       <c r="T106" s="20"/>
-    </row>
-    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U106">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="20">
         <v>1</v>
       </c>
@@ -12092,8 +12556,12 @@
         <v>0</v>
       </c>
       <c r="T107" s="20"/>
-    </row>
-    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U107">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="20">
         <v>1</v>
       </c>
@@ -12130,8 +12598,12 @@
         <v>0</v>
       </c>
       <c r="T108" s="20"/>
-    </row>
-    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U108">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="20"/>
       <c r="B109" s="20"/>
       <c r="C109" s="20"/>
@@ -12163,7 +12635,9 @@
       <c r="Q109" s="20">
         <v>2</v>
       </c>
-      <c r="R109" s="20"/>
+      <c r="R109" s="20">
+        <v>2</v>
+      </c>
       <c r="S109" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>74.680000000000007</v>
@@ -12171,8 +12645,12 @@
       <c r="T109" s="20" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U109">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="C110" s="20"/>
@@ -12209,8 +12687,12 @@
         <v>0</v>
       </c>
       <c r="T110" s="20"/>
-    </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U110">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="20"/>
       <c r="B111" s="20"/>
       <c r="C111" s="20"/>
@@ -12251,14 +12733,20 @@
       <c r="Q111" s="20">
         <v>15</v>
       </c>
-      <c r="R111" s="20"/>
+      <c r="R111" s="20">
+        <v>15</v>
+      </c>
       <c r="S111" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1.05</v>
       </c>
       <c r="T111" s="20"/>
-    </row>
-    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U111">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="20"/>
       <c r="B112" s="20"/>
       <c r="C112" s="20"/>
@@ -12303,8 +12791,12 @@
         <v>0</v>
       </c>
       <c r="T112" s="20"/>
-    </row>
-    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U112">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="20"/>
       <c r="B113" s="20"/>
       <c r="C113" s="20"/>
@@ -12349,8 +12841,12 @@
         <v>0</v>
       </c>
       <c r="T113" s="20"/>
-    </row>
-    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U113">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="20">
         <v>3</v>
       </c>
@@ -12378,15 +12874,23 @@
       <c r="P114" s="20">
         <v>0</v>
       </c>
-      <c r="Q114" s="20"/>
-      <c r="R114" s="20"/>
+      <c r="Q114" s="20">
+        <v>9</v>
+      </c>
+      <c r="R114" s="20">
+        <v>9</v>
+      </c>
       <c r="S114" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T114" s="20"/>
-    </row>
-    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U114">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
       <c r="B115" s="20"/>
       <c r="C115" s="20"/>
@@ -12427,8 +12931,12 @@
         <v>0</v>
       </c>
       <c r="T115" s="20"/>
-    </row>
-    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U115">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="20"/>
       <c r="B116" s="20"/>
       <c r="C116" s="20"/>
@@ -12461,14 +12969,20 @@
       <c r="Q116" s="20">
         <v>3</v>
       </c>
-      <c r="R116" s="20"/>
+      <c r="R116" s="20">
+        <v>3</v>
+      </c>
       <c r="S116" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T116" s="20"/>
-    </row>
-    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U116">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="20"/>
       <c r="B117" s="20"/>
       <c r="C117" s="20"/>
@@ -12509,8 +13023,12 @@
         <v>0</v>
       </c>
       <c r="T117" s="20"/>
-    </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U117">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="20"/>
       <c r="B118" s="20"/>
       <c r="C118" s="20"/>
@@ -12545,14 +13063,20 @@
       <c r="Q118" s="20">
         <v>6</v>
       </c>
-      <c r="R118" s="20"/>
+      <c r="R118" s="20">
+        <v>6</v>
+      </c>
       <c r="S118" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T118" s="20"/>
-    </row>
-    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U118">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="20"/>
       <c r="B119" s="20"/>
       <c r="C119" s="20"/>
@@ -12595,8 +13119,12 @@
         <v>0</v>
       </c>
       <c r="T119" s="20"/>
-    </row>
-    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U119">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" s="20"/>
       <c r="B120" s="20"/>
       <c r="C120" s="20"/>
@@ -12639,8 +13167,12 @@
         <v>0</v>
       </c>
       <c r="T120" s="20"/>
-    </row>
-    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U120">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="20"/>
       <c r="B121" s="20"/>
       <c r="C121" s="20"/>
@@ -12671,14 +13203,20 @@
       <c r="Q121" s="20">
         <v>6</v>
       </c>
-      <c r="R121" s="20"/>
+      <c r="R121" s="20">
+        <v>6</v>
+      </c>
       <c r="S121" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T121" s="20"/>
-    </row>
-    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U121">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" s="20"/>
       <c r="B122" s="20"/>
       <c r="C122" s="20"/>
@@ -12717,8 +13255,12 @@
         <v>0</v>
       </c>
       <c r="T122" s="20"/>
-    </row>
-    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U122">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" s="20"/>
       <c r="B123" s="20"/>
       <c r="C123" s="20"/>
@@ -12757,8 +13299,12 @@
         <v>0</v>
       </c>
       <c r="T123" s="20"/>
-    </row>
-    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U123">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" s="20"/>
       <c r="B124" s="20"/>
       <c r="C124" s="20"/>
@@ -12793,14 +13339,20 @@
       <c r="Q124" s="20">
         <v>6</v>
       </c>
-      <c r="R124" s="20"/>
+      <c r="R124" s="20">
+        <v>6</v>
+      </c>
       <c r="S124" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T124" s="20"/>
-    </row>
-    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U124">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" s="20"/>
       <c r="B125" s="20"/>
       <c r="C125" s="20"/>
@@ -12843,8 +13395,12 @@
         <v>0</v>
       </c>
       <c r="T125" s="20"/>
-    </row>
-    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U125">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" s="20"/>
       <c r="B126" s="20"/>
       <c r="C126" s="20"/>
@@ -12887,8 +13443,12 @@
         <v>0</v>
       </c>
       <c r="T126" s="20"/>
-    </row>
-    <row r="127" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U126">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127" s="20"/>
       <c r="B127" s="20"/>
       <c r="C127" s="20"/>
@@ -12923,14 +13483,20 @@
       <c r="Q127" s="20">
         <v>2</v>
       </c>
-      <c r="R127" s="20"/>
+      <c r="R127" s="20">
+        <v>2</v>
+      </c>
       <c r="S127" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T127" s="20"/>
-    </row>
-    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U127">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128" s="20"/>
       <c r="B128" s="20"/>
       <c r="C128" s="20"/>
@@ -12973,8 +13539,12 @@
         <v>0</v>
       </c>
       <c r="T128" s="20"/>
-    </row>
-    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U128">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129" s="20"/>
       <c r="B129" s="20"/>
       <c r="C129" s="20"/>
@@ -13017,8 +13587,12 @@
         <v>0</v>
       </c>
       <c r="T129" s="20"/>
-    </row>
-    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U129">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="20"/>
       <c r="B130" s="20"/>
       <c r="C130" s="20"/>
@@ -13055,8 +13629,12 @@
         <v>0</v>
       </c>
       <c r="T130" s="20"/>
-    </row>
-    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U130">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="20"/>
       <c r="B131" s="20"/>
       <c r="C131" s="20"/>
@@ -13093,8 +13671,12 @@
         <v>0</v>
       </c>
       <c r="T131" s="20"/>
-    </row>
-    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U131">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="20"/>
       <c r="B132" s="20"/>
       <c r="C132" s="20"/>
@@ -13131,8 +13713,12 @@
         <v>0</v>
       </c>
       <c r="T132" s="20"/>
-    </row>
-    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U132">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133" s="20">
         <v>1</v>
       </c>
@@ -13171,14 +13757,20 @@
       <c r="Q133" s="20">
         <v>3</v>
       </c>
-      <c r="R133" s="20"/>
+      <c r="R133" s="20">
+        <v>3</v>
+      </c>
       <c r="S133" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>127.80000000000001</v>
       </c>
       <c r="T133" s="20"/>
-    </row>
-    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U133">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134" s="20">
         <v>1</v>
       </c>
@@ -13221,8 +13813,12 @@
         <v>0</v>
       </c>
       <c r="T134" s="20"/>
-    </row>
-    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U134">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="20"/>
       <c r="B135" s="20"/>
       <c r="C135" s="20"/>
@@ -13259,8 +13855,12 @@
         <v>0</v>
       </c>
       <c r="T135" s="20"/>
-    </row>
-    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U135">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136" s="20"/>
       <c r="B136" s="20"/>
       <c r="C136" s="20"/>
@@ -13303,8 +13903,12 @@
         <v>0</v>
       </c>
       <c r="T136" s="20"/>
-    </row>
-    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U136">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137" s="20"/>
       <c r="B137" s="20"/>
       <c r="C137" s="20"/>
@@ -13347,8 +13951,12 @@
         <v>0</v>
       </c>
       <c r="T137" s="20"/>
-    </row>
-    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U137">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138" s="20"/>
       <c r="B138" s="20"/>
       <c r="C138" s="20"/>
@@ -13389,8 +13997,12 @@
         <v>0</v>
       </c>
       <c r="T138" s="20"/>
-    </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U138">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139" s="20"/>
       <c r="B139" s="20"/>
       <c r="C139" s="20"/>
@@ -13431,14 +14043,20 @@
       <c r="Q139" s="20">
         <v>10</v>
       </c>
-      <c r="R139" s="20"/>
+      <c r="R139" s="20">
+        <v>10</v>
+      </c>
       <c r="S139" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>7.1</v>
       </c>
       <c r="T139" s="20"/>
-    </row>
-    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U139">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A140" s="20">
         <v>7</v>
       </c>
@@ -13477,7 +14095,9 @@
       <c r="Q140" s="20">
         <v>25</v>
       </c>
-      <c r="R140" s="20"/>
+      <c r="R140" s="20">
+        <v>25</v>
+      </c>
       <c r="S140" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>8.25</v>
@@ -13485,8 +14105,12 @@
       <c r="T140" s="20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U140">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="20"/>
       <c r="B141" s="20"/>
       <c r="C141" s="20"/>
@@ -13523,8 +14147,12 @@
         <v>0</v>
       </c>
       <c r="T141" s="20"/>
-    </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U141">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A142" s="20"/>
       <c r="B142" s="20">
         <v>1</v>
@@ -13560,15 +14188,19 @@
         <v>6</v>
       </c>
       <c r="R142" s="20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S142" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T142" s="20"/>
-    </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U142">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A143" s="20">
         <v>2</v>
       </c>
@@ -13611,14 +14243,20 @@
       <c r="Q143" s="20">
         <v>5</v>
       </c>
-      <c r="R143" s="20"/>
+      <c r="R143" s="20">
+        <v>5</v>
+      </c>
       <c r="S143" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>16.968</v>
       </c>
       <c r="T143" s="20"/>
-    </row>
-    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U143">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144" s="20">
         <v>2</v>
       </c>
@@ -13663,8 +14301,12 @@
         <v>0</v>
       </c>
       <c r="T144" s="20"/>
-    </row>
-    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U144">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145" s="20">
         <v>2</v>
       </c>
@@ -13709,8 +14351,12 @@
         <v>0</v>
       </c>
       <c r="T145" s="20"/>
-    </row>
-    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U145">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A146" s="20">
         <v>2</v>
       </c>
@@ -13755,8 +14401,12 @@
         <v>0</v>
       </c>
       <c r="T146" s="20"/>
-    </row>
-    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U146">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A147" s="20">
         <v>2</v>
       </c>
@@ -13797,8 +14447,12 @@
         <v>0</v>
       </c>
       <c r="T147" s="20"/>
-    </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U147">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A148" s="20">
         <v>2</v>
       </c>
@@ -13839,14 +14493,20 @@
       <c r="Q148" s="20">
         <v>10</v>
       </c>
-      <c r="R148" s="20"/>
+      <c r="R148" s="20">
+        <v>10</v>
+      </c>
       <c r="S148" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>16.68</v>
       </c>
       <c r="T148" s="20"/>
-    </row>
-    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U148">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149" s="20">
         <v>2</v>
       </c>
@@ -13889,8 +14549,12 @@
         <v>0</v>
       </c>
       <c r="T149" s="20"/>
-    </row>
-    <row r="150" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U149">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150" s="20">
         <v>2</v>
       </c>
@@ -13929,8 +14593,12 @@
         <v>0</v>
       </c>
       <c r="T150" s="20"/>
-    </row>
-    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U150">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151" s="20"/>
       <c r="B151" s="20">
         <v>2</v>
@@ -13969,8 +14637,12 @@
         <v>0</v>
       </c>
       <c r="T151" s="20"/>
-    </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U151">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152" s="20"/>
       <c r="B152" s="20">
         <v>2</v>
@@ -14013,8 +14685,12 @@
         <v>0</v>
       </c>
       <c r="T152" s="20"/>
-    </row>
-    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U152">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="20"/>
       <c r="B153" s="20"/>
       <c r="C153" s="20"/>
@@ -14047,8 +14723,12 @@
         <v>0</v>
       </c>
       <c r="T153" s="20"/>
-    </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U153">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" s="20"/>
       <c r="B154" s="20"/>
       <c r="C154" s="20"/>
@@ -14085,14 +14765,20 @@
       <c r="Q154" s="20">
         <v>10</v>
       </c>
-      <c r="R154" s="20"/>
+      <c r="R154" s="20">
+        <v>10</v>
+      </c>
       <c r="S154" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0.59</v>
       </c>
       <c r="T154" s="20"/>
-    </row>
-    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U154">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="20"/>
       <c r="B155" s="20">
         <v>13</v>
@@ -14135,8 +14821,12 @@
         <v>0</v>
       </c>
       <c r="T155" s="20"/>
-    </row>
-    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U155">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="20"/>
       <c r="B156" s="20">
         <v>13</v>
@@ -14175,14 +14865,20 @@
       <c r="Q156" s="20">
         <v>50</v>
       </c>
-      <c r="R156" s="20"/>
+      <c r="R156" s="20">
+        <v>50</v>
+      </c>
       <c r="S156" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0.4</v>
       </c>
       <c r="T156" s="20"/>
-    </row>
-    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U156">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="20"/>
       <c r="B157" s="20">
         <v>13</v>
@@ -14221,8 +14917,12 @@
         <v>0</v>
       </c>
       <c r="T157" s="20"/>
-    </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U157">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" s="20"/>
       <c r="B158" s="20"/>
       <c r="C158" s="20"/>
@@ -14263,8 +14963,12 @@
         <v>0</v>
       </c>
       <c r="T158" s="20"/>
-    </row>
-    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U158">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="20"/>
       <c r="B159" s="20"/>
       <c r="C159" s="20"/>
@@ -14303,8 +15007,12 @@
         <v>0</v>
       </c>
       <c r="T159" s="20"/>
-    </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U159">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="20"/>
       <c r="B160" s="20"/>
       <c r="C160" s="20"/>
@@ -14345,8 +15053,12 @@
         <v>0</v>
       </c>
       <c r="T160" s="20"/>
-    </row>
-    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U160">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="20"/>
       <c r="B161" s="20"/>
       <c r="C161" s="20"/>
@@ -14383,8 +15095,12 @@
         <v>0</v>
       </c>
       <c r="T161" s="20"/>
-    </row>
-    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U161">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="20"/>
       <c r="B162" s="20">
         <v>35</v>
@@ -14429,8 +15145,12 @@
         <v>0</v>
       </c>
       <c r="T162" s="20"/>
-    </row>
-    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U162">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" s="20"/>
       <c r="B163" s="20">
         <v>35</v>
@@ -14471,14 +15191,20 @@
       <c r="Q163" s="20">
         <v>200</v>
       </c>
-      <c r="R163" s="20"/>
+      <c r="R163" s="20">
+        <v>200</v>
+      </c>
       <c r="S163" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>1.6</v>
       </c>
       <c r="T163" s="20"/>
-    </row>
-    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U163">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A164" s="20"/>
       <c r="B164" s="20">
         <v>35</v>
@@ -14521,8 +15247,12 @@
         <v>0</v>
       </c>
       <c r="T164" s="20"/>
-    </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U164">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165" s="20"/>
       <c r="B165" s="20"/>
       <c r="C165" s="20"/>
@@ -14563,8 +15293,12 @@
         <v>0</v>
       </c>
       <c r="T165" s="20"/>
-    </row>
-    <row r="166" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U165">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="20"/>
       <c r="B166" s="20"/>
       <c r="C166" s="20"/>
@@ -14605,8 +15339,12 @@
         <v>0</v>
       </c>
       <c r="T166" s="20"/>
-    </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U166">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167" s="20"/>
       <c r="B167" s="20"/>
       <c r="C167" s="20"/>
@@ -14647,8 +15385,12 @@
         <v>0</v>
       </c>
       <c r="T167" s="20"/>
-    </row>
-    <row r="168" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U167">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="20"/>
       <c r="B168" s="20"/>
       <c r="C168" s="20"/>
@@ -14689,8 +15431,12 @@
         <v>0</v>
       </c>
       <c r="T168" s="20"/>
-    </row>
-    <row r="169" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U168">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="20"/>
       <c r="B169" s="20"/>
       <c r="C169" s="20"/>
@@ -14731,8 +15477,12 @@
         <v>0</v>
       </c>
       <c r="T169" s="20"/>
-    </row>
-    <row r="170" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U169">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170" s="20"/>
       <c r="B170" s="20"/>
       <c r="C170" s="20"/>
@@ -14769,14 +15519,20 @@
       <c r="Q170" s="20">
         <v>50</v>
       </c>
-      <c r="R170" s="20"/>
+      <c r="R170" s="20">
+        <v>50</v>
+      </c>
       <c r="S170" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="T170" s="20"/>
-    </row>
-    <row r="171" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U170">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="20"/>
       <c r="B171" s="20"/>
       <c r="C171" s="20"/>
@@ -14817,8 +15573,12 @@
         <v>0</v>
       </c>
       <c r="T171" s="20"/>
-    </row>
-    <row r="172" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U171">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="20"/>
       <c r="B172" s="20"/>
       <c r="C172" s="20"/>
@@ -14859,8 +15619,12 @@
         <v>0</v>
       </c>
       <c r="T172" s="20"/>
-    </row>
-    <row r="173" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U172">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173" s="20"/>
       <c r="B173" s="20"/>
       <c r="C173" s="20"/>
@@ -14901,8 +15665,12 @@
         <v>0</v>
       </c>
       <c r="T173" s="20"/>
-    </row>
-    <row r="174" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U173">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" s="20"/>
       <c r="B174" s="20"/>
       <c r="C174" s="20"/>
@@ -14939,14 +15707,20 @@
       <c r="Q174" s="20">
         <v>50</v>
       </c>
-      <c r="R174" s="20"/>
+      <c r="R174" s="20">
+        <v>50</v>
+      </c>
       <c r="S174" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0.25</v>
       </c>
       <c r="T174" s="20"/>
-    </row>
-    <row r="175" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U174">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="20"/>
       <c r="B175" s="20"/>
       <c r="C175" s="20"/>
@@ -14987,8 +15761,12 @@
         <v>0</v>
       </c>
       <c r="T175" s="20"/>
-    </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U175">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="20"/>
       <c r="B176" s="20"/>
       <c r="C176" s="20"/>
@@ -15029,8 +15807,12 @@
         <v>0</v>
       </c>
       <c r="T176" s="20"/>
-    </row>
-    <row r="177" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U176">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="20"/>
       <c r="B177" s="20"/>
       <c r="C177" s="20"/>
@@ -15071,8 +15853,12 @@
         <v>0</v>
       </c>
       <c r="T177" s="20"/>
-    </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U177">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" s="20"/>
       <c r="B178" s="20"/>
       <c r="C178" s="20"/>
@@ -15113,8 +15899,12 @@
         <v>0</v>
       </c>
       <c r="T178" s="20"/>
-    </row>
-    <row r="179" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U178">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" s="20"/>
       <c r="B179" s="20"/>
       <c r="C179" s="20"/>
@@ -15149,8 +15939,12 @@
         <v>0</v>
       </c>
       <c r="T179" s="20"/>
-    </row>
-    <row r="180" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U179">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" s="20"/>
       <c r="B180" s="20"/>
       <c r="C180" s="20"/>
@@ -15187,14 +15981,20 @@
       <c r="Q180" s="20">
         <v>50</v>
       </c>
-      <c r="R180" s="20"/>
+      <c r="R180" s="20">
+        <v>50</v>
+      </c>
       <c r="S180" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="T180" s="20"/>
-    </row>
-    <row r="181" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U180">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181" s="20"/>
       <c r="B181" s="20"/>
       <c r="C181" s="20"/>
@@ -15235,8 +16035,12 @@
         <v>0</v>
       </c>
       <c r="T181" s="20"/>
-    </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U181">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" s="20"/>
       <c r="B182" s="20">
         <v>3</v>
@@ -15277,8 +16081,12 @@
         <v>0</v>
       </c>
       <c r="T182" s="20"/>
-    </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U182">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183" s="20">
         <v>1</v>
       </c>
@@ -15308,15 +16116,23 @@
       <c r="P183" s="20">
         <v>10</v>
       </c>
-      <c r="Q183" s="20"/>
-      <c r="R183" s="20"/>
+      <c r="Q183" s="20">
+        <v>10</v>
+      </c>
+      <c r="R183" s="20">
+        <v>9</v>
+      </c>
       <c r="S183" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T183" s="20"/>
-    </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U183">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" s="20">
         <v>1</v>
       </c>
@@ -15346,15 +16162,23 @@
       <c r="P184" s="20">
         <v>10</v>
       </c>
-      <c r="Q184" s="20"/>
-      <c r="R184" s="20"/>
+      <c r="Q184" s="20">
+        <v>10</v>
+      </c>
+      <c r="R184" s="20">
+        <v>10</v>
+      </c>
       <c r="S184" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T184" s="20"/>
-    </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U184">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185" s="20">
         <v>2</v>
       </c>
@@ -15384,15 +16208,23 @@
       <c r="P185" s="20">
         <v>10</v>
       </c>
-      <c r="Q185" s="20"/>
-      <c r="R185" s="20"/>
+      <c r="Q185" s="20">
+        <v>10</v>
+      </c>
+      <c r="R185" s="20">
+        <v>10</v>
+      </c>
       <c r="S185" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0</v>
       </c>
       <c r="T185" s="20"/>
-    </row>
-    <row r="186" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U185">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="20"/>
       <c r="B186" s="20"/>
       <c r="C186" s="20"/>
@@ -15429,8 +16261,12 @@
         <v>0</v>
       </c>
       <c r="T186" s="20"/>
-    </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U186">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187" s="20"/>
       <c r="B187" s="20"/>
       <c r="C187" s="20"/>
@@ -15466,14 +16302,20 @@
       <c r="Q187" s="20">
         <v>15</v>
       </c>
-      <c r="R187" s="20"/>
+      <c r="R187" s="20">
+        <v>5</v>
+      </c>
       <c r="S187" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>29.25</v>
       </c>
       <c r="T187" s="20"/>
-    </row>
-    <row r="188" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U187">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A188" s="20"/>
       <c r="B188" s="20"/>
       <c r="C188" s="20"/>
@@ -15514,8 +16356,12 @@
         <v>0</v>
       </c>
       <c r="T188" s="20"/>
-    </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U188">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189" s="20"/>
       <c r="B189" s="20"/>
       <c r="C189" s="20"/>
@@ -15550,14 +16396,20 @@
       <c r="Q189" s="20">
         <v>6</v>
       </c>
-      <c r="R189" s="20"/>
+      <c r="R189" s="20">
+        <v>6</v>
+      </c>
       <c r="S189" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>13.5</v>
       </c>
       <c r="T189" s="20"/>
-    </row>
-    <row r="190" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U189">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190" s="20"/>
       <c r="B190" s="20"/>
       <c r="C190" s="20"/>
@@ -15596,8 +16448,12 @@
         <v>0</v>
       </c>
       <c r="T190" s="20"/>
-    </row>
-    <row r="191" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U190">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191" s="20"/>
       <c r="B191" s="20"/>
       <c r="C191" s="20"/>
@@ -15634,8 +16490,12 @@
         <v>0</v>
       </c>
       <c r="T191" s="20"/>
-    </row>
-    <row r="192" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U191">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192" s="20"/>
       <c r="B192" s="20"/>
       <c r="C192" s="20"/>
@@ -15678,8 +16538,12 @@
         <v>0</v>
       </c>
       <c r="T192" s="20"/>
-    </row>
-    <row r="193" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U192">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193" s="20"/>
       <c r="B193" s="20"/>
       <c r="C193" s="20"/>
@@ -15718,14 +16582,20 @@
       <c r="Q193" s="20">
         <v>2</v>
       </c>
-      <c r="R193" s="20"/>
+      <c r="R193" s="20">
+        <v>2</v>
+      </c>
       <c r="S193" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>0.7</v>
       </c>
       <c r="T193" s="20"/>
-    </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U193">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194" s="20"/>
       <c r="B194" s="20"/>
       <c r="C194" s="20"/>
@@ -15766,14 +16636,20 @@
       <c r="Q194" s="20">
         <v>10</v>
       </c>
-      <c r="R194" s="20"/>
+      <c r="R194" s="20">
+        <v>10</v>
+      </c>
       <c r="S194" s="24">
         <f>Tableau5[[#This Row],[Quantité à commander]]*Tableau5[[#This Row],[Prix unitaire HT]]</f>
         <v>2.54</v>
       </c>
       <c r="T194" s="20"/>
-    </row>
-    <row r="195" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U194">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195" s="20"/>
       <c r="B195" s="20"/>
       <c r="C195" s="20"/>
@@ -15816,8 +16692,12 @@
         <v>0</v>
       </c>
       <c r="T195" s="20"/>
-    </row>
-    <row r="196" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U195">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="20"/>
       <c r="B196" s="20"/>
       <c r="C196" s="20"/>
@@ -15854,8 +16734,12 @@
         <v>0</v>
       </c>
       <c r="T196" s="20"/>
-    </row>
-    <row r="197" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U196">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A197" s="20"/>
       <c r="B197" s="20"/>
       <c r="C197" s="20"/>
@@ -15898,8 +16782,12 @@
         <v>0</v>
       </c>
       <c r="T197" s="20"/>
-    </row>
-    <row r="198" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U197">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A198" s="20"/>
       <c r="B198" s="20"/>
       <c r="C198" s="20"/>
@@ -15944,8 +16832,12 @@
         <v>0</v>
       </c>
       <c r="T198" s="20"/>
-    </row>
-    <row r="199" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U198">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A199" s="20"/>
       <c r="B199" s="20"/>
       <c r="C199" s="20"/>
@@ -15969,6 +16861,10 @@
         <v>0</v>
       </c>
       <c r="T199" s="20"/>
+      <c r="U199">
+        <f>Tableau5[[#This Row],[Quantité commandée]]-Tableau5[[#This Row],[Quantité reçue]]</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17158,7 +18054,7 @@
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>

</xml_diff>